<commit_message>
clean up and restructuring of repo
</commit_message>
<xml_diff>
--- a/clockshift/sumrule_analysis_results.xlsx
+++ b/clockshift/sumrule_analysis_results.xlsx
@@ -438,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BU6"/>
+  <dimension ref="A1:BU8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1948,6 +1948,460 @@
         <v>1.960112051461479</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2024-09-12_E_e.dat</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>transfer</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>200</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Blackman</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>0.447</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.0028</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.0148</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.00055</v>
+      </c>
+      <c r="I7" t="n">
+        <v>10818242.33717204</v>
+      </c>
+      <c r="J7" t="n">
+        <v>377</v>
+      </c>
+      <c r="K7" t="n">
+        <v>13</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="M7" t="n">
+        <v>1.353251525585472</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0.01823642281480822</v>
+      </c>
+      <c r="O7" t="n">
+        <v>3.384760825824527</v>
+      </c>
+      <c r="P7" t="n">
+        <v>0.04561305003519604</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>268.9189189189189</v>
+      </c>
+      <c r="R7" t="n">
+        <v>42.68013515262911</v>
+      </c>
+      <c r="S7" t="n">
+        <v>0.597685403414816</v>
+      </c>
+      <c r="T7" t="n">
+        <v>0.3098666670904903</v>
+      </c>
+      <c r="U7" t="n">
+        <v>0.01836981553431876</v>
+      </c>
+      <c r="V7" t="n">
+        <v>0.3473690933134114</v>
+      </c>
+      <c r="W7" t="n">
+        <v>2.176582100597987</v>
+      </c>
+      <c r="X7" t="n">
+        <v>0.3282364826248091</v>
+      </c>
+      <c r="Y7" t="n">
+        <v>2.523951193911398</v>
+      </c>
+      <c r="Z7" t="n">
+        <v>7.689429199728545</v>
+      </c>
+      <c r="AA7" t="n">
+        <v>0.2348580854810282</v>
+      </c>
+      <c r="AB7" t="n">
+        <v>0.01013078014731138</v>
+      </c>
+      <c r="AC7" t="n">
+        <v>0.3373026864360487</v>
+      </c>
+      <c r="AD7" t="n">
+        <v>0.344974735785374</v>
+      </c>
+      <c r="AE7" t="n">
+        <v>0.3298719555730663</v>
+      </c>
+      <c r="AF7" t="n">
+        <v>0.3374450992921992</v>
+      </c>
+      <c r="AG7" t="n">
+        <v>0.008089328022197521</v>
+      </c>
+      <c r="AH7" t="n">
+        <v>2.650770589112001</v>
+      </c>
+      <c r="AI7" t="n">
+        <v>2.70922255528005</v>
+      </c>
+      <c r="AJ7" t="n">
+        <v>2.581354759869761</v>
+      </c>
+      <c r="AK7" t="n">
+        <v>2.646708965697791</v>
+      </c>
+      <c r="AL7" t="n">
+        <v>0.06443938461543329</v>
+      </c>
+      <c r="AM7" t="n">
+        <v>7.862530888593243</v>
+      </c>
+      <c r="AN7" t="n">
+        <v>8.071431991609899</v>
+      </c>
+      <c r="AO7" t="n">
+        <v>7.621923052448456</v>
+      </c>
+      <c r="AP7" t="n">
+        <v>7.846747444082977</v>
+      </c>
+      <c r="AQ7" t="n">
+        <v>0.232870309309199</v>
+      </c>
+      <c r="AR7" t="n">
+        <v>0.01943038952938295</v>
+      </c>
+      <c r="AS7" t="n">
+        <v>0.01991282363412602</v>
+      </c>
+      <c r="AT7" t="n">
+        <v>0.01886497187300008</v>
+      </c>
+      <c r="AU7" t="n">
+        <v>0.01939564278916637</v>
+      </c>
+      <c r="AV7" t="n">
+        <v>0.000526360150116652</v>
+      </c>
+      <c r="AW7" t="n">
+        <v>2.302253037201362</v>
+      </c>
+      <c r="AX7" t="n">
+        <v>2.359176934236709</v>
+      </c>
+      <c r="AY7" t="n">
+        <v>2.235269316893389</v>
+      </c>
+      <c r="AZ7" t="n">
+        <v>2.297922443227667</v>
+      </c>
+      <c r="BA7" t="n">
+        <v>0.06207740544018735</v>
+      </c>
+      <c r="BB7" t="n">
+        <v>0.3486887782037926</v>
+      </c>
+      <c r="BC7" t="n">
+        <v>0.3563837980805823</v>
+      </c>
+      <c r="BD7" t="n">
+        <v>0.3405055953707706</v>
+      </c>
+      <c r="BE7" t="n">
+        <v>0.3487865224701245</v>
+      </c>
+      <c r="BF7" t="n">
+        <v>0.008845137064875557</v>
+      </c>
+      <c r="BG7" t="n">
+        <v>1.454080806710048</v>
+      </c>
+      <c r="BH7" t="n">
+        <v>1.490033447924836</v>
+      </c>
+      <c r="BI7" t="n">
+        <v>1.411775459226118</v>
+      </c>
+      <c r="BJ7" t="n">
+        <v>1.451328557431822</v>
+      </c>
+      <c r="BK7" t="n">
+        <v>0.03920150396585813</v>
+      </c>
+      <c r="BL7" t="n">
+        <v>2.15540550673144</v>
+      </c>
+      <c r="BM7" t="n">
+        <v>2.219596836482521</v>
+      </c>
+      <c r="BN7" t="n">
+        <v>2.082332307800371</v>
+      </c>
+      <c r="BO7" t="n">
+        <v>2.151459300582226</v>
+      </c>
+      <c r="BP7" t="n">
+        <v>0.07072926319807023</v>
+      </c>
+      <c r="BQ7" t="n">
+        <v>3.630071685653816</v>
+      </c>
+      <c r="BR7" t="n">
+        <v>0.09805103665383658</v>
+      </c>
+      <c r="BS7" t="n">
+        <v>3.636955628042732</v>
+      </c>
+      <c r="BT7" t="n">
+        <v>3.726880589713171</v>
+      </c>
+      <c r="BU7" t="n">
+        <v>3.531141239380172</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2024-09-18_F_e.dat</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>transfer</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>200</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Blackman</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>0.6889999999999999</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.009900000000000001</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.0186</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.00014</v>
+      </c>
+      <c r="I8" t="n">
+        <v>12127808.20404177</v>
+      </c>
+      <c r="J8" t="n">
+        <v>377</v>
+      </c>
+      <c r="K8" t="n">
+        <v>13</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0.7663633636591822</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0.01823642281480822</v>
+      </c>
+      <c r="O8" t="n">
+        <v>1.709852237829378</v>
+      </c>
+      <c r="P8" t="n">
+        <v>0.0406877335719948</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>213.9784946236559</v>
+      </c>
+      <c r="R8" t="n">
+        <v>136.2503920113797</v>
+      </c>
+      <c r="S8" t="n">
+        <v>6.091112189062183</v>
+      </c>
+      <c r="T8" t="n">
+        <v>0.8170872608259792</v>
+      </c>
+      <c r="U8" t="n">
+        <v>0.003384662392636809</v>
+      </c>
+      <c r="V8" t="n">
+        <v>0.03696083600119154</v>
+      </c>
+      <c r="W8" t="n">
+        <v>0.7362064422805231</v>
+      </c>
+      <c r="X8" t="n">
+        <v>0.820471923218616</v>
+      </c>
+      <c r="Y8" t="n">
+        <v>0.7731672782817146</v>
+      </c>
+      <c r="Z8" t="n">
+        <v>0.9423445902312773</v>
+      </c>
+      <c r="AA8" t="n">
+        <v>0.4698072715794814</v>
+      </c>
+      <c r="AB8" t="n">
+        <v>0.01653871829921932</v>
+      </c>
+      <c r="AC8" t="n">
+        <v>0.351763617729176</v>
+      </c>
+      <c r="AD8" t="n">
+        <v>0.3669817794881653</v>
+      </c>
+      <c r="AE8" t="n">
+        <v>0.3376683775226238</v>
+      </c>
+      <c r="AF8" t="n">
+        <v>0.3521845749111452</v>
+      </c>
+      <c r="AG8" t="n">
+        <v>0.01373476543499438</v>
+      </c>
+      <c r="AH8" t="n">
+        <v>0.9557550836038384</v>
+      </c>
+      <c r="AI8" t="n">
+        <v>0.9891662673434409</v>
+      </c>
+      <c r="AJ8" t="n">
+        <v>0.9236846561540357</v>
+      </c>
+      <c r="AK8" t="n">
+        <v>0.9549304444654596</v>
+      </c>
+      <c r="AL8" t="n">
+        <v>0.03260395484408993</v>
+      </c>
+      <c r="AM8" t="n">
+        <v>2.711787530709346</v>
+      </c>
+      <c r="AN8" t="n">
+        <v>2.873109813708927</v>
+      </c>
+      <c r="AO8" t="n">
+        <v>2.572900857329363</v>
+      </c>
+      <c r="AP8" t="n">
+        <v>2.715749851987404</v>
+      </c>
+      <c r="AQ8" t="n">
+        <v>0.1440443472497804</v>
+      </c>
+      <c r="AR8" t="n">
+        <v>0.003631281234409604</v>
+      </c>
+      <c r="AS8" t="n">
+        <v>0.003779725136137824</v>
+      </c>
+      <c r="AT8" t="n">
+        <v>0.003485725796355147</v>
+      </c>
+      <c r="AU8" t="n">
+        <v>0.003630970176366508</v>
+      </c>
+      <c r="AV8" t="n">
+        <v>0.0001448439314680616</v>
+      </c>
+      <c r="AW8" t="n">
+        <v>0.7898508346236919</v>
+      </c>
+      <c r="AX8" t="n">
+        <v>0.8221388795426557</v>
+      </c>
+      <c r="AY8" t="n">
+        <v>0.7581913840172039</v>
+      </c>
+      <c r="AZ8" t="n">
+        <v>0.7897833767657624</v>
+      </c>
+      <c r="BA8" t="n">
+        <v>0.0315054717437733</v>
+      </c>
+      <c r="BB8" t="n">
+        <v>0.1653459088236783</v>
+      </c>
+      <c r="BC8" t="n">
+        <v>0.1715149702597857</v>
+      </c>
+      <c r="BD8" t="n">
+        <v>0.1578411112170259</v>
+      </c>
+      <c r="BE8" t="n">
+        <v>0.1651470676996971</v>
+      </c>
+      <c r="BF8" t="n">
+        <v>0.006795520846426978</v>
+      </c>
+      <c r="BG8" t="n">
+        <v>0.6490102675788103</v>
+      </c>
+      <c r="BH8" t="n">
+        <v>0.6755408578834345</v>
+      </c>
+      <c r="BI8" t="n">
+        <v>0.6229962442106776</v>
+      </c>
+      <c r="BJ8" t="n">
+        <v>0.6489548759671027</v>
+      </c>
+      <c r="BK8" t="n">
+        <v>0.02588764734473556</v>
+      </c>
+      <c r="BL8" t="n">
+        <v>0.9231716820827645</v>
+      </c>
+      <c r="BM8" t="n">
+        <v>0.9786291849319789</v>
+      </c>
+      <c r="BN8" t="n">
+        <v>0.8705223432078169</v>
+      </c>
+      <c r="BO8" t="n">
+        <v>0.9227996727485688</v>
+      </c>
+      <c r="BP8" t="n">
+        <v>0.05271334586028383</v>
+      </c>
+      <c r="BQ8" t="n">
+        <v>1.447899259725191</v>
+      </c>
+      <c r="BR8" t="n">
+        <v>0.05775856968577506</v>
+      </c>
+      <c r="BS8" t="n">
+        <v>1.448022845318822</v>
+      </c>
+      <c r="BT8" t="n">
+        <v>1.507215900929803</v>
+      </c>
+      <c r="BU8" t="n">
+        <v>1.38998231496444</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>